<commit_message>
Fixing one instance of Competition
</commit_message>
<xml_diff>
--- a/knowledge-graph/competitions.xlsx
+++ b/knowledge-graph/competitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Projects\ISWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Projects\ISWS\project-implementation\knowledge-graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D49545-B8AC-4CCF-A63C-EBFA37A4644E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAB2857-A62E-4B81-BADC-B2545CE56434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{C9484112-5D4A-4635-8C27-F9A778E4EE0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{C9484112-5D4A-4635-8C27-F9A778E4EE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="3" r:id="rId1"/>
@@ -296,9 +296,6 @@
     <t>T010</t>
   </si>
   <si>
-    <t>onto-ind:USA</t>
-  </si>
-  <si>
     <t>onto-ind:T001</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>onto-ind:F</t>
+  </si>
+  <si>
+    <t>onto-ind:AUS</t>
   </si>
 </sst>
 </file>
@@ -795,10 +795,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +854,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DEFB84-3835-4E6C-A8BF-47AB8E008CFC}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,10 +1007,10 @@
         <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,10 +1024,10 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,10 +1041,10 @@
         <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,10 +1058,10 @@
         <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,10 +1075,10 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,10 +1092,10 @@
         <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,10 +1109,10 @@
         <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,10 +1126,10 @@
         <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,10 +1143,10 @@
         <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,10 +1160,10 @@
         <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,10 +1177,10 @@
         <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1193,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5A0E5C-8E1B-4D59-9BBD-F285259C2F4F}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1258,10 @@
         <v>64</v>
       </c>
       <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
         <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>86</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>20</v>
@@ -1284,13 +1284,13 @@
         <v>44835</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>25</v>
@@ -1316,10 +1316,10 @@
         <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>28</v>
@@ -1345,10 +1345,10 @@
         <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>35</v>
@@ -1374,10 +1374,10 @@
         <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>28</v>
@@ -1411,18 +1411,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
         <v>102</v>
       </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>